<commit_message>
motive analysis phase 1
</commit_message>
<xml_diff>
--- a/Data/murder(2016-2021)/STATE-UT wise murder data(2021-2015)reg.xlsx
+++ b/Data/murder(2016-2021)/STATE-UT wise murder data(2021-2015)reg.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="STATE-UT wise murder data(2021-" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>m_p_pop</t>
   </si>
 </sst>
 </file>
@@ -963,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +979,7 @@
     <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1010,8 +1013,11 @@
       <c r="L1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1048,8 +1054,12 @@
       <c r="L2">
         <v>1.768</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>(D2+E2+F2+G2+H2+I2+J2)/(L2*7)</f>
+        <v>560.35875888817066</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1086,8 +1096,12 @@
       <c r="L3">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f t="shared" ref="M3:M37" si="0">(D3+E3+F3+G3+H3+I3+J3)/(L3*7)</f>
+        <v>185.25345622119815</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1124,8 +1138,12 @@
       <c r="L4">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>3891.2442396313363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1162,8 +1180,12 @@
       <c r="L5">
         <v>1.5960000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>1842.8213390619405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1200,8 +1222,12 @@
       <c r="L6">
         <v>2.1539999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>440.64199495954375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1238,8 +1264,12 @@
       <c r="L7">
         <v>1.2090000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>25.759187049509627</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1276,8 +1306,12 @@
       <c r="L8">
         <v>1.2090000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>871.44038756941973</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1314,8 +1348,12 @@
       <c r="L9">
         <v>1.024</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>1063.4765625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1352,8 +1390,12 @@
       <c r="L10">
         <v>1.024</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>91.378348214285708</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1390,8 +1432,12 @@
       <c r="L11">
         <v>1.5960000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>989.52738990332966</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1428,8 +1474,12 @@
       <c r="L12">
         <v>1.768</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>804.54104718810606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1466,8 +1516,12 @@
       <c r="L13">
         <v>1.768</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>179.62184873949582</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1504,8 +1558,12 @@
       <c r="L14">
         <v>2.1539999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>935.26992969889909</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1542,8 +1600,12 @@
       <c r="L15">
         <v>1.2090000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>1871.0859033439676</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1580,8 +1642,12 @@
       <c r="L16">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>204.14746543778801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1618,8 +1684,12 @@
       <c r="L17">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>308.29493087557603</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1656,8 +1726,12 @@
       <c r="L18">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>92.626728110599075</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1694,8 +1768,12 @@
       <c r="L19">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>109.67741935483872</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1732,8 +1810,12 @@
       <c r="L20">
         <v>1.5960000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>866.72037235947005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1770,8 +1852,12 @@
       <c r="L21">
         <v>1.024</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>699.77678571428567</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1808,8 +1894,12 @@
       <c r="L22">
         <v>1.024</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>1574.3582589285713</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1846,8 +1936,12 @@
       <c r="L23">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>46.543778801843317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1884,8 +1978,12 @@
       <c r="L24">
         <v>1.768</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>942.065287653523</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1922,8 +2020,12 @@
       <c r="L25">
         <v>1.768</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>526.26050420168065</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1960,8 +2062,12 @@
       <c r="L26">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>431.33640552995394</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1998,8 +2104,12 @@
       <c r="L27">
         <v>2.1539999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>1949.3964716805942</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2036,8 +2146,12 @@
       <c r="L28">
         <v>2.1539999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>89.202812044037671</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2074,8 +2188,12 @@
       <c r="L29">
         <v>1.5960000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>1241.7651271034729</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2112,8 +2230,12 @@
       <c r="L30">
         <v>1.768</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>7.0297349709114414</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2150,8 +2272,12 @@
       <c r="L31">
         <v>1.024</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>22.321428571428569</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2188,8 +2314,12 @@
       <c r="L32">
         <v>1.2090000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>9.4529126787191284</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2226,8 +2356,12 @@
       <c r="L33">
         <v>1.024</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>499.16294642857144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2264,8 +2398,12 @@
       <c r="L34">
         <v>1.024</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>146.20535714285714</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2290,8 +2428,12 @@
       <c r="L35">
         <v>1.024</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>0.69754464285714279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2328,8 +2470,12 @@
       <c r="L36">
         <v>1.768</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <f t="shared" si="0"/>
+        <v>0.16160310277957338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2365,6 +2511,10 @@
       </c>
       <c r="L37">
         <v>1.768</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>16.725921137685845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>